<commit_message>
Update on input example files Update on airplane definition Airplane general data importation Selection of sheets imported implemented Table log erros Correction on delete instance (stretche foreign keys)
</commit_message>
<xml_diff>
--- a/Input example files/Airplanes.xlsx
+++ b/Input example files/Airplanes.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Airplane" sheetId="1" r:id="rId1"/>
+    <sheet name="Airplanes" sheetId="1" r:id="rId1"/>
     <sheet name="Seat List" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Model</t>
   </si>
@@ -56,6 +56,96 @@
   </si>
   <si>
     <t>Max Luggage Weight</t>
+  </si>
+  <si>
+    <t>5H-BAD</t>
+  </si>
+  <si>
+    <t>5H-BAT</t>
+  </si>
+  <si>
+    <t>5H-BEE</t>
+  </si>
+  <si>
+    <t>5H-EGG</t>
+  </si>
+  <si>
+    <t>5H-FED</t>
+  </si>
+  <si>
+    <t>5H-GUS</t>
+  </si>
+  <si>
+    <t>5H-HOT</t>
+  </si>
+  <si>
+    <t>5H-JOE</t>
+  </si>
+  <si>
+    <t>5H-LUV</t>
+  </si>
+  <si>
+    <t>5H-LXJ</t>
+  </si>
+  <si>
+    <t>5H-MAD</t>
+  </si>
+  <si>
+    <t>5H-NHB</t>
+  </si>
+  <si>
+    <t>5H-OJF</t>
+  </si>
+  <si>
+    <t>5H-POA</t>
+  </si>
+  <si>
+    <t>5H-RJS</t>
+  </si>
+  <si>
+    <t>5H-SUN</t>
+  </si>
+  <si>
+    <t>5H-VIP</t>
+  </si>
+  <si>
+    <t>5H-ZEB</t>
+  </si>
+  <si>
+    <t>5H-FAB</t>
+  </si>
+  <si>
+    <t>5H-JAM</t>
+  </si>
+  <si>
+    <t>5H-LEO</t>
+  </si>
+  <si>
+    <t>5H-MAG</t>
+  </si>
+  <si>
+    <t>Cessna Caravan-208B</t>
+  </si>
+  <si>
+    <t>Pilatus PC12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dar Es Salaam </t>
+  </si>
+  <si>
+    <t>Dar Es Salaam</t>
+  </si>
+  <si>
+    <t>Arusha</t>
+  </si>
+  <si>
+    <t>Fuel Burn 1st hr</t>
+  </si>
+  <si>
+    <t>Fuel Burn 2nd Hr</t>
+  </si>
+  <si>
+    <t>Max Fuel</t>
   </si>
 </sst>
 </file>
@@ -93,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -116,11 +206,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -128,6 +229,12 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,21 +515,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.88671875" style="2"/>
     <col min="5" max="5" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -446,6 +556,785 @@
       </c>
       <c r="H1" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D2" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E2" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F2" s="9">
+        <v>150</v>
+      </c>
+      <c r="G2" s="10">
+        <v>12</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="8">
+        <v>350</v>
+      </c>
+      <c r="J2" s="8">
+        <v>330</v>
+      </c>
+      <c r="K2" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D3" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E3" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F3" s="9">
+        <v>150</v>
+      </c>
+      <c r="G3" s="10">
+        <v>12</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="8">
+        <v>350</v>
+      </c>
+      <c r="J3" s="8">
+        <v>330</v>
+      </c>
+      <c r="K3" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F4" s="9">
+        <v>150</v>
+      </c>
+      <c r="G4" s="10">
+        <v>12</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="8">
+        <v>350</v>
+      </c>
+      <c r="J4" s="8">
+        <v>330</v>
+      </c>
+      <c r="K4" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F5" s="9">
+        <v>150</v>
+      </c>
+      <c r="G5" s="10">
+        <v>12</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="8">
+        <v>350</v>
+      </c>
+      <c r="J5" s="8">
+        <v>330</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D6" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E6" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F6" s="9">
+        <v>150</v>
+      </c>
+      <c r="G6" s="10">
+        <v>12</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="8">
+        <v>350</v>
+      </c>
+      <c r="J6" s="8">
+        <v>330</v>
+      </c>
+      <c r="K6" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F7" s="9">
+        <v>150</v>
+      </c>
+      <c r="G7" s="10">
+        <v>12</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="8">
+        <v>350</v>
+      </c>
+      <c r="J7" s="8">
+        <v>330</v>
+      </c>
+      <c r="K7" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F8" s="9">
+        <v>150</v>
+      </c>
+      <c r="G8" s="10">
+        <v>12</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="8">
+        <v>350</v>
+      </c>
+      <c r="J8" s="8">
+        <v>330</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D9" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F9" s="9">
+        <v>150</v>
+      </c>
+      <c r="G9" s="10">
+        <v>12</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="8">
+        <v>350</v>
+      </c>
+      <c r="J9" s="8">
+        <v>330</v>
+      </c>
+      <c r="K9" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E10" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F10" s="9">
+        <v>150</v>
+      </c>
+      <c r="G10" s="10">
+        <v>12</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="8">
+        <v>350</v>
+      </c>
+      <c r="J10" s="8">
+        <v>330</v>
+      </c>
+      <c r="K10" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F11" s="9">
+        <v>150</v>
+      </c>
+      <c r="G11" s="10">
+        <v>12</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="8">
+        <v>350</v>
+      </c>
+      <c r="J11" s="8">
+        <v>330</v>
+      </c>
+      <c r="K11" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F12" s="9">
+        <v>150</v>
+      </c>
+      <c r="G12" s="10">
+        <v>12</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="8">
+        <v>350</v>
+      </c>
+      <c r="J12" s="8">
+        <v>330</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E13" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F13" s="9">
+        <v>150</v>
+      </c>
+      <c r="G13" s="10">
+        <v>12</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="8">
+        <v>350</v>
+      </c>
+      <c r="J13" s="8">
+        <v>330</v>
+      </c>
+      <c r="K13" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E14" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F14" s="9">
+        <v>150</v>
+      </c>
+      <c r="G14" s="10">
+        <v>12</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="8">
+        <v>350</v>
+      </c>
+      <c r="J14" s="8">
+        <v>330</v>
+      </c>
+      <c r="K14" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E15" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F15" s="9">
+        <v>150</v>
+      </c>
+      <c r="G15" s="10">
+        <v>12</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="8">
+        <v>350</v>
+      </c>
+      <c r="J15" s="8">
+        <v>330</v>
+      </c>
+      <c r="K15" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D16" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E16" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F16" s="9">
+        <v>150</v>
+      </c>
+      <c r="G16" s="10">
+        <v>12</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="8">
+        <v>350</v>
+      </c>
+      <c r="J16" s="8">
+        <v>330</v>
+      </c>
+      <c r="K16" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E17" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F17" s="9">
+        <v>150</v>
+      </c>
+      <c r="G17" s="10">
+        <v>12</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="8">
+        <v>350</v>
+      </c>
+      <c r="J17" s="8">
+        <v>330</v>
+      </c>
+      <c r="K17" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D18" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E18" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F18" s="9">
+        <v>150</v>
+      </c>
+      <c r="G18" s="10">
+        <v>12</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="8">
+        <v>350</v>
+      </c>
+      <c r="J18" s="8">
+        <v>330</v>
+      </c>
+      <c r="K18" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1982</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2073</v>
+      </c>
+      <c r="E19" s="9">
+        <v>3967</v>
+      </c>
+      <c r="F19" s="9">
+        <v>150</v>
+      </c>
+      <c r="G19" s="10">
+        <v>12</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="8">
+        <v>350</v>
+      </c>
+      <c r="J19" s="8">
+        <v>330</v>
+      </c>
+      <c r="K19" s="8">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="9">
+        <v>2804</v>
+      </c>
+      <c r="D20" s="9">
+        <v>2761</v>
+      </c>
+      <c r="E20" s="9">
+        <v>4740</v>
+      </c>
+      <c r="F20" s="9">
+        <v>220</v>
+      </c>
+      <c r="G20" s="10">
+        <v>9</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="8">
+        <v>450</v>
+      </c>
+      <c r="J20" s="8">
+        <v>330</v>
+      </c>
+      <c r="K20" s="8">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2804</v>
+      </c>
+      <c r="D21" s="9">
+        <v>2761</v>
+      </c>
+      <c r="E21" s="9">
+        <v>4740</v>
+      </c>
+      <c r="F21" s="9">
+        <v>220</v>
+      </c>
+      <c r="G21" s="10">
+        <v>9</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="8">
+        <v>450</v>
+      </c>
+      <c r="J21" s="8">
+        <v>330</v>
+      </c>
+      <c r="K21" s="8">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2804</v>
+      </c>
+      <c r="D22" s="9">
+        <v>2761</v>
+      </c>
+      <c r="E22" s="9">
+        <v>4740</v>
+      </c>
+      <c r="F22" s="9">
+        <v>220</v>
+      </c>
+      <c r="G22" s="10">
+        <v>9</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="8">
+        <v>450</v>
+      </c>
+      <c r="J22" s="8">
+        <v>330</v>
+      </c>
+      <c r="K22" s="8">
+        <v>2737</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2804</v>
+      </c>
+      <c r="D23" s="9">
+        <v>2761</v>
+      </c>
+      <c r="E23" s="9">
+        <v>4740</v>
+      </c>
+      <c r="F23" s="9">
+        <v>220</v>
+      </c>
+      <c r="G23" s="10">
+        <v>9</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="8">
+        <v>450</v>
+      </c>
+      <c r="J23" s="8">
+        <v>330</v>
+      </c>
+      <c r="K23" s="8">
+        <v>2737</v>
       </c>
     </row>
   </sheetData>
@@ -458,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA1E913-F630-4546-ACB8-EF1AA2802EDE}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Correction on seat list importation Correction on visualization of data about optimization on status bar
</commit_message>
<xml_diff>
--- a/Input example files/Airplanes.xlsx
+++ b/Input example files/Airplanes.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834C2CA2-5DBF-48E6-8F0C-B10FEAC133E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
@@ -50,9 +51,6 @@
   </si>
   <si>
     <t>Class</t>
-  </si>
-  <si>
-    <t>Number of seats</t>
   </si>
   <si>
     <t>Max Luggage Weight</t>
@@ -227,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -240,8 +238,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,21 +561,21 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8">
         <v>1982</v>
@@ -597,7 +593,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" s="7">
         <v>350</v>
@@ -611,10 +607,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8">
         <v>1982</v>
@@ -632,7 +628,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" s="7">
         <v>350</v>
@@ -646,10 +642,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8">
         <v>1982</v>
@@ -667,7 +663,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" s="7">
         <v>350</v>
@@ -681,10 +677,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="8">
         <v>1982</v>
@@ -702,7 +698,7 @@
         <v>12</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="7">
         <v>350</v>
@@ -716,10 +712,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="8">
         <v>1982</v>
@@ -737,7 +733,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="7">
         <v>350</v>
@@ -751,10 +747,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="8">
         <v>1982</v>
@@ -772,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="7">
         <v>350</v>
@@ -786,10 +782,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="8">
         <v>1982</v>
@@ -807,7 +803,7 @@
         <v>12</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="7">
         <v>350</v>
@@ -821,10 +817,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8">
         <v>1982</v>
@@ -842,7 +838,7 @@
         <v>12</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" s="7">
         <v>350</v>
@@ -856,10 +852,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="8">
         <v>1982</v>
@@ -877,7 +873,7 @@
         <v>12</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="7">
         <v>350</v>
@@ -891,10 +887,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="8">
         <v>1982</v>
@@ -912,7 +908,7 @@
         <v>12</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11" s="7">
         <v>350</v>
@@ -926,10 +922,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="8">
         <v>1982</v>
@@ -947,7 +943,7 @@
         <v>12</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" s="7">
         <v>350</v>
@@ -961,10 +957,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="8">
         <v>1982</v>
@@ -982,7 +978,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="7">
         <v>350</v>
@@ -996,10 +992,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="8">
         <v>1982</v>
@@ -1017,7 +1013,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" s="7">
         <v>350</v>
@@ -1031,10 +1027,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="8">
         <v>1982</v>
@@ -1052,7 +1048,7 @@
         <v>12</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I15" s="7">
         <v>350</v>
@@ -1066,10 +1062,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="8">
         <v>1982</v>
@@ -1087,7 +1083,7 @@
         <v>12</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I16" s="7">
         <v>350</v>
@@ -1101,10 +1097,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="8">
         <v>1982</v>
@@ -1122,7 +1118,7 @@
         <v>12</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I17" s="7">
         <v>350</v>
@@ -1136,10 +1132,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="8">
         <v>1982</v>
@@ -1157,7 +1153,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I18" s="7">
         <v>350</v>
@@ -1171,10 +1167,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="8">
         <v>1982</v>
@@ -1192,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I19" s="7">
         <v>350</v>
@@ -1206,10 +1202,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8">
         <v>2804</v>
@@ -1227,7 +1223,7 @@
         <v>9</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" s="7">
         <v>450</v>
@@ -1241,10 +1237,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="8">
         <v>2804</v>
@@ -1262,7 +1258,7 @@
         <v>9</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="7">
         <v>450</v>
@@ -1276,10 +1272,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="8">
         <v>2804</v>
@@ -1297,7 +1293,7 @@
         <v>9</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I22" s="7">
         <v>450</v>
@@ -1311,10 +1307,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="8">
         <v>2804</v>
@@ -1332,7 +1328,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I23" s="7">
         <v>450</v>
@@ -1352,646 +1348,510 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA1E913-F630-4546-ACB8-EF1AA2802EDE}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="14.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="9">
-        <v>8</v>
-      </c>
-      <c r="D2" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="C2" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="9">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C3" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="9">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="B6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="9">
-        <v>8</v>
-      </c>
-      <c r="D6" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="B8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="9">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="9">
-        <v>8</v>
-      </c>
-      <c r="D8" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>15</v>
-      </c>
       <c r="B9" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="9">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C9" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="9">
-        <v>10</v>
-      </c>
-      <c r="D10" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="B12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="9">
-        <v>2</v>
-      </c>
-      <c r="D11" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="B13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="9">
-        <v>8</v>
-      </c>
-      <c r="D12" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="B14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="9">
-        <v>4</v>
-      </c>
-      <c r="D13" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="B15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="9">
-        <v>8</v>
-      </c>
-      <c r="D14" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="B16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="9">
-        <v>4</v>
-      </c>
-      <c r="D15" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="B17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="9">
-        <v>8</v>
-      </c>
-      <c r="D16" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="B18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="9">
-        <v>4</v>
-      </c>
-      <c r="D17" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="B19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="9">
-        <v>10</v>
-      </c>
-      <c r="D18" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="B20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="9">
-        <v>2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="B21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="9">
-        <v>10</v>
-      </c>
-      <c r="D20" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="B22" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="9">
-        <v>2</v>
-      </c>
-      <c r="D21" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="B23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="9">
-        <v>8</v>
-      </c>
-      <c r="D22" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="B24" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="9">
-        <v>4</v>
-      </c>
-      <c r="D23" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="B25" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="9">
-        <v>8</v>
-      </c>
-      <c r="D24" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="B26" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="9">
-        <v>4</v>
-      </c>
-      <c r="D25" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="B27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="9">
-        <v>8</v>
-      </c>
-      <c r="D26" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="B28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="9">
-        <v>4</v>
-      </c>
-      <c r="D27" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="B29" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="9">
-        <v>6</v>
-      </c>
-      <c r="D28" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="B30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="9">
-        <v>6</v>
-      </c>
-      <c r="D29" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="B31" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="9">
-        <v>6</v>
-      </c>
-      <c r="D30" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+      <c r="B32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="9">
-        <v>6</v>
-      </c>
-      <c r="D31" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="B33" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="9">
-        <v>10</v>
-      </c>
-      <c r="D32" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="B34" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C33" s="9">
-        <v>2</v>
-      </c>
-      <c r="D33" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="B35" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="9">
-        <v>8</v>
-      </c>
-      <c r="D34" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="B36" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="9">
-        <v>4</v>
-      </c>
-      <c r="D35" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="B37" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="9">
-        <v>8</v>
-      </c>
-      <c r="D36" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="B38" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="9">
-        <v>4</v>
-      </c>
-      <c r="D37" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="9">
-        <v>3</v>
-      </c>
-      <c r="D38" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="B39" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="9">
-        <v>6</v>
-      </c>
-      <c r="D39" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C39" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="9">
-        <v>4</v>
-      </c>
-      <c r="D40" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+      <c r="B42" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="9">
-        <v>5</v>
-      </c>
-      <c r="D41" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="B43" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="9">
-        <v>2</v>
-      </c>
-      <c r="D42" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="B44" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="9">
-        <v>7</v>
-      </c>
-      <c r="D43" s="7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="9">
-        <v>5</v>
-      </c>
-      <c r="D44" s="7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="B45" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C45" s="9">
-        <v>4</v>
-      </c>
-      <c r="D45" s="7">
+        <v>42</v>
+      </c>
+      <c r="C45" s="7">
         <v>30</v>
       </c>
     </row>

</xml_diff>